<commit_message>
Deploying to gh-pages from  @ 2a7cab7092f35db58b1834153938a85b0f5652c1 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/3.4.2.xlsx
+++ b/en/downloads/data-excel/3.4.2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="47">
   <si>
     <t>Кыргызская Республика</t>
   </si>
@@ -142,6 +142,30 @@
   <si>
     <t>3.4.2 Suicide mortality rate</t>
   </si>
+  <si>
+    <t>эркектер</t>
+  </si>
+  <si>
+    <t>мужчины</t>
+  </si>
+  <si>
+    <t> men</t>
+  </si>
+  <si>
+    <t>аялдар</t>
+  </si>
+  <si>
+    <t>женщины</t>
+  </si>
+  <si>
+    <t> women</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>women</t>
+  </si>
 </sst>
 </file>
 
@@ -152,7 +176,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _р_._-;\-* #,##0.00\ _р_._-;_-* &quot;-&quot;??\ _р_._-;_-@_-"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +294,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -345,7 +377,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -359,12 +391,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -381,9 +407,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -396,55 +419,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="19"/>
@@ -458,6 +439,26 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Normal 17" xfId="18"/>
@@ -8249,7 +8250,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8263,10 +8264,10 @@
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D1" s="2"/>
@@ -8282,17 +8283,17 @@
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -8304,10 +8305,10 @@
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A3" s="9"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="35"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="18"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -8319,699 +8320,1926 @@
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="16">
         <v>2007</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="16">
         <v>2008</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="16">
         <v>2009</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="16">
         <v>2010</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="16">
         <v>2011</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="16">
         <v>2012</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="16">
         <v>2013</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="16">
         <v>2014</v>
       </c>
-      <c r="L4" s="24">
+      <c r="L4" s="16">
         <v>2015</v>
       </c>
-      <c r="M4" s="25">
+      <c r="M4" s="16">
         <v>2016</v>
       </c>
-      <c r="N4" s="25">
+      <c r="N4" s="16">
         <v>2017</v>
       </c>
-      <c r="O4" s="25">
+      <c r="O4" s="16">
         <v>2018</v>
       </c>
-      <c r="P4" s="25">
+      <c r="P4" s="16">
         <v>2019</v>
       </c>
-      <c r="Q4" s="25">
+      <c r="Q4" s="16">
         <v>2020</v>
       </c>
-      <c r="R4" s="25">
+      <c r="R4" s="16">
         <v>2021</v>
       </c>
-      <c r="S4" s="25">
+      <c r="S4" s="16">
         <v>2022</v>
       </c>
-      <c r="T4" s="25">
+      <c r="T4" s="16">
         <v>2023</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="16.5" customHeight="1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>9.1999999999999993</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="25">
         <v>8.9</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="25">
         <v>8.5</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="25">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H5" s="25">
         <v>8.5</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="25">
         <v>9.3000000000000007</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J5" s="25">
         <v>7.8</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="25">
         <v>7.9</v>
       </c>
-      <c r="L5" s="26">
+      <c r="L5" s="25">
         <v>7</v>
       </c>
-      <c r="M5" s="26">
+      <c r="M5" s="25">
         <v>6.9</v>
       </c>
-      <c r="N5" s="27">
+      <c r="N5" s="21">
         <v>6.3</v>
       </c>
-      <c r="O5" s="34">
+      <c r="O5" s="21">
         <v>6</v>
       </c>
-      <c r="P5" s="34">
+      <c r="P5" s="21">
         <v>5.8</v>
       </c>
-      <c r="Q5" s="34">
+      <c r="Q5" s="21">
         <v>4.5999999999999996</v>
       </c>
-      <c r="R5" s="34">
+      <c r="R5" s="21">
         <v>5.8</v>
       </c>
-      <c r="S5" s="38">
+      <c r="S5" s="21">
         <v>4.9000000000000004</v>
       </c>
-      <c r="T5" s="38">
+      <c r="T5" s="21">
         <v>4.8</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:20" s="29" customFormat="1">
+      <c r="A6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="27">
+        <v>14.2</v>
+      </c>
+      <c r="E6" s="27">
+        <v>14.4</v>
+      </c>
+      <c r="F6" s="27">
+        <v>13.6</v>
+      </c>
+      <c r="G6" s="27">
+        <v>14.7</v>
+      </c>
+      <c r="H6" s="27">
+        <v>13.3</v>
+      </c>
+      <c r="I6" s="27">
+        <v>14.5</v>
+      </c>
+      <c r="J6" s="27">
+        <v>12.3</v>
+      </c>
+      <c r="K6" s="27">
+        <v>12.4</v>
+      </c>
+      <c r="L6" s="27">
+        <v>11.1</v>
+      </c>
+      <c r="M6" s="27">
+        <v>11</v>
+      </c>
+      <c r="N6" s="22">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="O6" s="22">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="P6" s="22">
+        <v>9.4</v>
+      </c>
+      <c r="Q6" s="22">
+        <v>7.1</v>
+      </c>
+      <c r="R6" s="22">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="S6" s="22">
+        <v>8.1</v>
+      </c>
+      <c r="T6" s="22">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" s="29" customFormat="1">
+      <c r="A7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="27">
+        <v>4.3</v>
+      </c>
+      <c r="E7" s="27">
+        <v>3.5</v>
+      </c>
+      <c r="F7" s="27">
+        <v>3.5</v>
+      </c>
+      <c r="G7" s="27">
+        <v>3.8</v>
+      </c>
+      <c r="H7" s="27">
+        <v>3.9</v>
+      </c>
+      <c r="I7" s="27">
+        <v>4.3</v>
+      </c>
+      <c r="J7" s="27">
+        <v>3.4</v>
+      </c>
+      <c r="K7" s="27">
+        <v>3.5</v>
+      </c>
+      <c r="L7" s="27">
+        <v>3</v>
+      </c>
+      <c r="M7" s="27">
+        <v>2.9</v>
+      </c>
+      <c r="N7" s="22">
+        <v>2.5</v>
+      </c>
+      <c r="O7" s="22">
+        <v>2.4</v>
+      </c>
+      <c r="P7" s="22">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q7" s="22">
+        <v>2.1</v>
+      </c>
+      <c r="R7" s="22">
+        <v>2.8</v>
+      </c>
+      <c r="S7" s="22">
+        <v>1.8</v>
+      </c>
+      <c r="T7" s="22">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="30" customFormat="1">
+      <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B8" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D8" s="25">
         <v>6.6</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E8" s="25">
         <v>8.5</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F8" s="25">
         <v>7.4</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G8" s="25">
         <v>6.4</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H8" s="25">
         <v>8.5</v>
       </c>
-      <c r="I6" s="28">
+      <c r="I8" s="25">
         <v>9.6999999999999993</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J8" s="25">
         <v>6.9</v>
       </c>
-      <c r="K6" s="28">
+      <c r="K8" s="25">
         <v>6.1</v>
       </c>
-      <c r="L6" s="28">
+      <c r="L8" s="25">
         <v>8.1999999999999993</v>
       </c>
-      <c r="M6" s="28">
+      <c r="M8" s="25">
         <v>5.8</v>
       </c>
-      <c r="N6" s="29">
+      <c r="N8" s="21">
         <v>6.1</v>
       </c>
-      <c r="O6" s="29">
+      <c r="O8" s="21">
         <v>7.5</v>
       </c>
-      <c r="P6" s="30">
+      <c r="P8" s="21">
         <v>6.8</v>
       </c>
-      <c r="Q6" s="30">
+      <c r="Q8" s="21">
         <v>4.2</v>
       </c>
-      <c r="R6" s="30">
+      <c r="R8" s="21">
         <v>4.7</v>
       </c>
-      <c r="S6" s="39">
+      <c r="S8" s="21">
         <v>3.4</v>
       </c>
-      <c r="T6" s="39">
+      <c r="T8" s="21">
         <v>5.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="28">
-        <v>5.7</v>
-      </c>
-      <c r="E7" s="28">
-        <v>4.7</v>
-      </c>
-      <c r="F7" s="28">
-        <v>2.4</v>
-      </c>
-      <c r="G7" s="28">
-        <v>1.5</v>
-      </c>
-      <c r="H7" s="28">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="I7" s="28">
-        <v>3.8</v>
-      </c>
-      <c r="J7" s="28">
-        <v>2.8</v>
-      </c>
-      <c r="K7" s="28">
-        <v>3.9</v>
-      </c>
-      <c r="L7" s="28">
-        <v>2.7</v>
-      </c>
-      <c r="M7" s="28">
-        <v>2.9</v>
-      </c>
-      <c r="N7" s="29">
-        <v>1.4</v>
-      </c>
-      <c r="O7" s="29">
-        <v>1.5</v>
-      </c>
-      <c r="P7" s="30">
-        <v>2.6</v>
-      </c>
-      <c r="Q7" s="30">
-        <v>1.3</v>
-      </c>
-      <c r="R7" s="30">
-        <v>1.6</v>
-      </c>
-      <c r="S7" s="39">
-        <v>3.5</v>
-      </c>
-      <c r="T7" s="39">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="A8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="28">
-        <v>20</v>
-      </c>
-      <c r="E8" s="28">
-        <v>21.5</v>
-      </c>
-      <c r="F8" s="28">
-        <v>21.2</v>
-      </c>
-      <c r="G8" s="28">
-        <v>23</v>
-      </c>
-      <c r="H8" s="28">
-        <v>22</v>
-      </c>
-      <c r="I8" s="28">
-        <v>25.1</v>
-      </c>
-      <c r="J8" s="28">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="K8" s="28">
-        <v>21</v>
-      </c>
-      <c r="L8" s="28">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="M8" s="28">
-        <v>15.6</v>
-      </c>
-      <c r="N8" s="30">
-        <v>15</v>
-      </c>
-      <c r="O8" s="30">
-        <v>19.5</v>
-      </c>
-      <c r="P8" s="30">
-        <v>15.6</v>
-      </c>
-      <c r="Q8" s="30">
-        <v>10.8</v>
-      </c>
-      <c r="R8" s="30">
-        <v>12.9</v>
-      </c>
-      <c r="S8" s="39">
-        <v>13.1</v>
-      </c>
-      <c r="T8" s="39">
-        <v>8.9</v>
       </c>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="28">
-        <v>14.8</v>
-      </c>
-      <c r="E9" s="28">
-        <v>16.3</v>
-      </c>
-      <c r="F9" s="28">
-        <v>15.5</v>
-      </c>
-      <c r="G9" s="28">
-        <v>19.2</v>
-      </c>
-      <c r="H9" s="28">
-        <v>16.7</v>
-      </c>
-      <c r="I9" s="28">
-        <v>14.6</v>
-      </c>
-      <c r="J9" s="28">
-        <v>13</v>
-      </c>
-      <c r="K9" s="28">
-        <v>17.2</v>
-      </c>
-      <c r="L9" s="28">
-        <v>13.8</v>
-      </c>
-      <c r="M9" s="28">
-        <v>13.2</v>
-      </c>
-      <c r="N9" s="29">
-        <v>15.2</v>
-      </c>
-      <c r="O9" s="29">
+      <c r="A9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="27">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="E9" s="27">
+        <v>13.4</v>
+      </c>
+      <c r="F9" s="27">
+        <v>9.1</v>
+      </c>
+      <c r="G9" s="27">
+        <v>7.6</v>
+      </c>
+      <c r="H9" s="27">
+        <v>13.3</v>
+      </c>
+      <c r="I9" s="27">
+        <v>14.3</v>
+      </c>
+      <c r="J9" s="27">
         <v>10.199999999999999</v>
       </c>
-      <c r="P9" s="30">
-        <v>10.4</v>
-      </c>
-      <c r="Q9" s="30">
-        <v>6.5</v>
-      </c>
-      <c r="R9" s="30">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="S9" s="39">
-        <v>8.1</v>
-      </c>
-      <c r="T9" s="39">
-        <v>11.9</v>
+      <c r="K9" s="27">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="L9" s="27">
+        <v>10.9</v>
+      </c>
+      <c r="M9" s="27">
+        <v>9.5</v>
+      </c>
+      <c r="N9" s="22">
+        <v>8.9</v>
+      </c>
+      <c r="O9" s="22">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="P9" s="22">
+        <v>9.6</v>
+      </c>
+      <c r="Q9" s="22">
+        <v>5.8</v>
+      </c>
+      <c r="R9" s="22">
+        <v>4.3</v>
+      </c>
+      <c r="S9" s="22">
+        <v>4.2</v>
+      </c>
+      <c r="T9" s="22">
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="28">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E10" s="28">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="F10" s="28">
-        <v>4.5</v>
-      </c>
-      <c r="G10" s="28">
-        <v>4.2</v>
-      </c>
-      <c r="H10" s="28">
+      <c r="A10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="27">
+        <v>3.9</v>
+      </c>
+      <c r="E10" s="27">
+        <v>3.4</v>
+      </c>
+      <c r="F10" s="27">
+        <v>5.7</v>
+      </c>
+      <c r="G10" s="27">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H10" s="27">
+        <v>3.7</v>
+      </c>
+      <c r="I10" s="27">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J10" s="27">
+        <v>3.5</v>
+      </c>
+      <c r="K10" s="27">
+        <v>3.9</v>
+      </c>
+      <c r="L10" s="27">
+        <v>5.4</v>
+      </c>
+      <c r="M10" s="27">
+        <v>2</v>
+      </c>
+      <c r="N10" s="22">
+        <v>3.2</v>
+      </c>
+      <c r="O10" s="22">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="P10" s="22">
+        <v>3.8</v>
+      </c>
+      <c r="Q10" s="22">
+        <v>2.6</v>
+      </c>
+      <c r="R10" s="22">
+        <v>5.2</v>
+      </c>
+      <c r="S10" s="22">
+        <v>2.5</v>
+      </c>
+      <c r="T10" s="22">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" s="30" customFormat="1">
+      <c r="A11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="25">
+        <v>5.7</v>
+      </c>
+      <c r="E11" s="25">
         <v>4.7</v>
       </c>
-      <c r="I10" s="28">
-        <v>5.3</v>
-      </c>
-      <c r="J10" s="28">
-        <v>6.2</v>
-      </c>
-      <c r="K10" s="28">
-        <v>5.8</v>
-      </c>
-      <c r="L10" s="28">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="M10" s="28">
+      <c r="F11" s="25">
+        <v>2.4</v>
+      </c>
+      <c r="G11" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="H11" s="25">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I11" s="25">
+        <v>3.8</v>
+      </c>
+      <c r="J11" s="25">
+        <v>2.8</v>
+      </c>
+      <c r="K11" s="25">
         <v>3.9</v>
       </c>
-      <c r="N10" s="29">
-        <v>3.8</v>
-      </c>
-      <c r="O10" s="29">
+      <c r="L11" s="25">
+        <v>2.7</v>
+      </c>
+      <c r="M11" s="25">
         <v>2.9</v>
       </c>
-      <c r="P10" s="30">
+      <c r="N11" s="21">
+        <v>1.4</v>
+      </c>
+      <c r="O11" s="21">
+        <v>1.5</v>
+      </c>
+      <c r="P11" s="21">
+        <v>2.6</v>
+      </c>
+      <c r="Q11" s="21">
+        <v>1.3</v>
+      </c>
+      <c r="R11" s="21">
+        <v>1.6</v>
+      </c>
+      <c r="S11" s="21">
         <v>3.5</v>
       </c>
-      <c r="Q10" s="30">
-        <v>2.9</v>
-      </c>
-      <c r="R10" s="30">
-        <v>4.2</v>
-      </c>
-      <c r="S10" s="39">
-        <v>2.5</v>
-      </c>
-      <c r="T10" s="39">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="28">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="E11" s="28">
-        <v>4</v>
-      </c>
-      <c r="F11" s="28">
-        <v>7.5</v>
-      </c>
-      <c r="G11" s="28">
-        <v>7.8</v>
-      </c>
-      <c r="H11" s="28">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="I11" s="28">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="J11" s="28">
-        <v>12.4</v>
-      </c>
-      <c r="K11" s="28">
-        <v>6.1</v>
-      </c>
-      <c r="L11" s="28">
-        <v>8.4</v>
-      </c>
-      <c r="M11" s="28">
-        <v>4.3</v>
-      </c>
-      <c r="N11" s="29">
-        <v>3.1</v>
-      </c>
-      <c r="O11" s="29">
-        <v>3.8</v>
-      </c>
-      <c r="P11" s="30">
-        <v>3</v>
-      </c>
-      <c r="Q11" s="30">
-        <v>2.6</v>
-      </c>
-      <c r="R11" s="30">
-        <v>3.3</v>
-      </c>
-      <c r="S11" s="39">
-        <v>2.6</v>
-      </c>
-      <c r="T11" s="39">
-        <v>0.7</v>
+      <c r="T11" s="21">
+        <v>1.9</v>
       </c>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="28">
-        <v>15.8</v>
-      </c>
-      <c r="E12" s="28">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="F12" s="28">
-        <v>17.8</v>
-      </c>
-      <c r="G12" s="28">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="H12" s="28">
-        <v>17.2</v>
-      </c>
-      <c r="I12" s="28">
-        <v>20.5</v>
-      </c>
-      <c r="J12" s="28">
-        <v>14.2</v>
-      </c>
-      <c r="K12" s="28">
-        <v>14.4</v>
-      </c>
-      <c r="L12" s="28">
-        <v>13.8</v>
-      </c>
-      <c r="M12" s="28">
-        <v>16.7</v>
-      </c>
-      <c r="N12" s="29">
-        <v>15.2</v>
-      </c>
-      <c r="O12" s="29">
-        <v>13.7</v>
-      </c>
-      <c r="P12" s="30">
-        <v>11.6</v>
-      </c>
-      <c r="Q12" s="30">
-        <v>13.1</v>
-      </c>
-      <c r="R12" s="30">
-        <v>15.2</v>
-      </c>
-      <c r="S12" s="39">
-        <v>10.8</v>
-      </c>
-      <c r="T12" s="39">
-        <v>12.7</v>
+      <c r="A12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="27">
+        <v>9.9</v>
+      </c>
+      <c r="E12" s="27">
+        <v>6.8</v>
+      </c>
+      <c r="F12" s="27">
+        <v>3.9</v>
+      </c>
+      <c r="G12" s="27">
+        <v>2.9</v>
+      </c>
+      <c r="H12" s="27">
+        <v>2.9</v>
+      </c>
+      <c r="I12" s="27">
+        <v>5.6</v>
+      </c>
+      <c r="J12" s="27">
+        <v>4.2</v>
+      </c>
+      <c r="K12" s="27">
+        <v>5</v>
+      </c>
+      <c r="L12" s="27">
+        <v>4.2</v>
+      </c>
+      <c r="M12" s="27">
+        <v>4</v>
+      </c>
+      <c r="N12" s="22">
+        <v>2</v>
+      </c>
+      <c r="O12" s="22">
+        <v>1.8</v>
+      </c>
+      <c r="P12" s="22">
+        <v>3.9</v>
+      </c>
+      <c r="Q12" s="22">
+        <v>2.1</v>
+      </c>
+      <c r="R12" s="22">
+        <v>1.9</v>
+      </c>
+      <c r="S12" s="22">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="T12" s="22">
+        <v>3.2</v>
       </c>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="28">
-        <v>10.3</v>
-      </c>
-      <c r="E13" s="28">
-        <v>5.3</v>
-      </c>
-      <c r="F13" s="28">
-        <v>5.7</v>
-      </c>
-      <c r="G13" s="28">
-        <v>8.6</v>
-      </c>
-      <c r="H13" s="28">
-        <v>6.5</v>
-      </c>
-      <c r="I13" s="28">
-        <v>4.2</v>
-      </c>
-      <c r="J13" s="28">
-        <v>3.8</v>
-      </c>
-      <c r="K13" s="28">
-        <v>3.2</v>
-      </c>
-      <c r="L13" s="28">
+      <c r="A13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="27">
+        <v>1.4</v>
+      </c>
+      <c r="E13" s="27">
+        <v>2.6</v>
+      </c>
+      <c r="F13" s="27">
+        <v>0.8</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="27">
+        <v>1.7</v>
+      </c>
+      <c r="I13" s="27">
+        <v>1.9</v>
+      </c>
+      <c r="J13" s="27">
+        <v>1.5</v>
+      </c>
+      <c r="K13" s="27">
+        <v>2.7</v>
+      </c>
+      <c r="L13" s="27">
+        <v>1.2</v>
+      </c>
+      <c r="M13" s="27">
+        <v>1.9</v>
+      </c>
+      <c r="N13" s="22">
+        <v>0.9</v>
+      </c>
+      <c r="O13" s="22">
+        <v>1.2</v>
+      </c>
+      <c r="P13" s="22">
+        <v>1.3</v>
+      </c>
+      <c r="Q13" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="R13" s="22">
+        <v>1.3</v>
+      </c>
+      <c r="S13" s="22">
         <v>2.5</v>
       </c>
-      <c r="M13" s="28">
-        <v>2.8</v>
-      </c>
-      <c r="N13" s="29">
-        <v>2.4</v>
-      </c>
-      <c r="O13" s="29">
-        <v>1.8</v>
-      </c>
-      <c r="P13" s="30">
-        <v>2.6</v>
-      </c>
-      <c r="Q13" s="30">
-        <v>1</v>
-      </c>
-      <c r="R13" s="30">
-        <v>2.4</v>
-      </c>
-      <c r="S13" s="39">
-        <v>2.1</v>
-      </c>
-      <c r="T13" s="39">
-        <v>1.1000000000000001</v>
+      <c r="T13" s="22">
+        <v>0.6</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A14" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="31">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E14" s="31">
-        <v>3.9</v>
-      </c>
-      <c r="F14" s="31">
-        <v>4.3</v>
-      </c>
-      <c r="G14" s="31">
-        <v>1.6</v>
-      </c>
-      <c r="H14" s="31">
-        <v>1.6</v>
-      </c>
-      <c r="I14" s="31">
-        <v>2.7</v>
-      </c>
-      <c r="J14" s="31">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K14" s="31">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="L14" s="31">
-        <v>1.8</v>
-      </c>
-      <c r="M14" s="31">
-        <v>2.5</v>
-      </c>
-      <c r="N14" s="32">
-        <v>2.5</v>
-      </c>
-      <c r="O14" s="32">
-        <v>1.7</v>
-      </c>
-      <c r="P14" s="37">
-        <v>2.9</v>
-      </c>
-      <c r="Q14" s="37">
-        <v>1.3</v>
-      </c>
-      <c r="R14" s="37">
-        <v>0.6</v>
-      </c>
-      <c r="S14" s="37">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="T14" s="37">
-        <v>2.2000000000000002</v>
+    <row r="14" spans="1:20" s="30" customFormat="1">
+      <c r="A14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="25">
+        <v>20</v>
+      </c>
+      <c r="E14" s="25">
+        <v>21.5</v>
+      </c>
+      <c r="F14" s="25">
+        <v>21.2</v>
+      </c>
+      <c r="G14" s="25">
+        <v>23</v>
+      </c>
+      <c r="H14" s="25">
+        <v>22</v>
+      </c>
+      <c r="I14" s="25">
+        <v>25.1</v>
+      </c>
+      <c r="J14" s="25">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="K14" s="25">
+        <v>21</v>
+      </c>
+      <c r="L14" s="25">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="M14" s="25">
+        <v>15.6</v>
+      </c>
+      <c r="N14" s="21">
+        <v>15</v>
+      </c>
+      <c r="O14" s="21">
+        <v>19.5</v>
+      </c>
+      <c r="P14" s="21">
+        <v>15.6</v>
+      </c>
+      <c r="Q14" s="21">
+        <v>10.8</v>
+      </c>
+      <c r="R14" s="21">
+        <v>12.9</v>
+      </c>
+      <c r="S14" s="21">
+        <v>13.1</v>
+      </c>
+      <c r="T14" s="21">
+        <v>8.9</v>
       </c>
     </row>
     <row r="15" spans="1:20">
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
+      <c r="A15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="27">
+        <v>29.9</v>
+      </c>
+      <c r="E15" s="27">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="F15" s="27">
+        <v>34.5</v>
+      </c>
+      <c r="G15" s="27">
+        <v>37</v>
+      </c>
+      <c r="H15" s="27">
+        <v>34.4</v>
+      </c>
+      <c r="I15" s="27">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="J15" s="27">
+        <v>31.8</v>
+      </c>
+      <c r="K15" s="27">
+        <v>34.5</v>
+      </c>
+      <c r="L15" s="27">
+        <v>29.7</v>
+      </c>
+      <c r="M15" s="27">
+        <v>24.2</v>
+      </c>
+      <c r="N15" s="22">
+        <v>25.5</v>
+      </c>
+      <c r="O15" s="22">
+        <v>32.6</v>
+      </c>
+      <c r="P15" s="22">
+        <v>22</v>
+      </c>
+      <c r="Q15" s="22">
+        <v>18.5</v>
+      </c>
+      <c r="R15" s="22">
+        <v>20.7</v>
+      </c>
+      <c r="S15" s="22">
+        <v>23.2</v>
+      </c>
+      <c r="T15" s="22">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="27">
+        <v>10.4</v>
+      </c>
+      <c r="E16" s="27">
+        <v>8.6</v>
+      </c>
+      <c r="F16" s="27">
+        <v>8.1</v>
+      </c>
+      <c r="G16" s="27">
+        <v>9.4</v>
+      </c>
+      <c r="H16" s="27">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I16" s="27">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="J16" s="27">
+        <v>6.5</v>
+      </c>
+      <c r="K16" s="27">
+        <v>7.8</v>
+      </c>
+      <c r="L16" s="27">
+        <v>5.5</v>
+      </c>
+      <c r="M16" s="27">
+        <v>7.1</v>
+      </c>
+      <c r="N16" s="22">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="O16" s="22">
+        <v>6.6</v>
+      </c>
+      <c r="P16" s="22">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="Q16" s="22">
+        <v>3.2</v>
+      </c>
+      <c r="R16" s="22">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="S16" s="22">
+        <v>3</v>
+      </c>
+      <c r="T16" s="22">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" s="30" customFormat="1">
+      <c r="A17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="25">
+        <v>14.8</v>
+      </c>
+      <c r="E17" s="25">
+        <v>16.3</v>
+      </c>
+      <c r="F17" s="25">
+        <v>15.5</v>
+      </c>
+      <c r="G17" s="25">
+        <v>19.2</v>
+      </c>
+      <c r="H17" s="25">
+        <v>16.7</v>
+      </c>
+      <c r="I17" s="25">
+        <v>14.6</v>
+      </c>
+      <c r="J17" s="25">
+        <v>13</v>
+      </c>
+      <c r="K17" s="25">
+        <v>17.2</v>
+      </c>
+      <c r="L17" s="25">
+        <v>13.8</v>
+      </c>
+      <c r="M17" s="25">
+        <v>13.2</v>
+      </c>
+      <c r="N17" s="21">
+        <v>15.2</v>
+      </c>
+      <c r="O17" s="21">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="P17" s="21">
+        <v>10.4</v>
+      </c>
+      <c r="Q17" s="21">
+        <v>6.5</v>
+      </c>
+      <c r="R17" s="21">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="S17" s="21">
+        <v>8.1</v>
+      </c>
+      <c r="T17" s="21">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="27">
+        <v>23.9</v>
+      </c>
+      <c r="E18" s="27">
+        <v>28.5</v>
+      </c>
+      <c r="F18" s="27">
+        <v>24.5</v>
+      </c>
+      <c r="G18" s="27">
+        <v>29.5</v>
+      </c>
+      <c r="H18" s="27">
+        <v>27.7</v>
+      </c>
+      <c r="I18" s="27">
+        <v>24.4</v>
+      </c>
+      <c r="J18" s="27">
+        <v>21.2</v>
+      </c>
+      <c r="K18" s="27">
+        <v>28.2</v>
+      </c>
+      <c r="L18" s="27">
+        <v>20.7</v>
+      </c>
+      <c r="M18" s="27">
+        <v>19.7</v>
+      </c>
+      <c r="N18" s="22">
+        <v>25.8</v>
+      </c>
+      <c r="O18" s="22">
+        <v>16.5</v>
+      </c>
+      <c r="P18" s="22">
+        <v>15.7</v>
+      </c>
+      <c r="Q18" s="22">
+        <v>11.5</v>
+      </c>
+      <c r="R18" s="22">
+        <v>16.7</v>
+      </c>
+      <c r="S18" s="22">
+        <v>13.5</v>
+      </c>
+      <c r="T18" s="22">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="27">
+        <v>5.5</v>
+      </c>
+      <c r="E19" s="27">
+        <v>3.9</v>
+      </c>
+      <c r="F19" s="27">
+        <v>6.3</v>
+      </c>
+      <c r="G19" s="27">
+        <v>8.5</v>
+      </c>
+      <c r="H19" s="27">
+        <v>5.4</v>
+      </c>
+      <c r="I19" s="27">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J19" s="27">
+        <v>4.5</v>
+      </c>
+      <c r="K19" s="27">
+        <v>5.9</v>
+      </c>
+      <c r="L19" s="27">
+        <v>6.6</v>
+      </c>
+      <c r="M19" s="27">
+        <v>6.5</v>
+      </c>
+      <c r="N19" s="22">
+        <v>4.3</v>
+      </c>
+      <c r="O19" s="22">
+        <v>3.6</v>
+      </c>
+      <c r="P19" s="22">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Q19" s="22">
+        <v>1.4</v>
+      </c>
+      <c r="R19" s="22">
+        <v>3.5</v>
+      </c>
+      <c r="S19" s="22">
+        <v>2.6</v>
+      </c>
+      <c r="T19" s="22">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" s="30" customFormat="1">
+      <c r="A20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="25">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E20" s="25">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F20" s="25">
+        <v>4.5</v>
+      </c>
+      <c r="G20" s="25">
+        <v>4.2</v>
+      </c>
+      <c r="H20" s="25">
+        <v>4.7</v>
+      </c>
+      <c r="I20" s="25">
+        <v>5.3</v>
+      </c>
+      <c r="J20" s="25">
+        <v>6.2</v>
+      </c>
+      <c r="K20" s="25">
+        <v>5.8</v>
+      </c>
+      <c r="L20" s="25">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M20" s="25">
+        <v>3.9</v>
+      </c>
+      <c r="N20" s="21">
+        <v>3.8</v>
+      </c>
+      <c r="O20" s="21">
+        <v>2.9</v>
+      </c>
+      <c r="P20" s="21">
+        <v>3.5</v>
+      </c>
+      <c r="Q20" s="21">
+        <v>2.9</v>
+      </c>
+      <c r="R20" s="21">
+        <v>4.2</v>
+      </c>
+      <c r="S20" s="21">
+        <v>2.5</v>
+      </c>
+      <c r="T20" s="21">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="27">
+        <v>5.9</v>
+      </c>
+      <c r="E21" s="27">
+        <v>7.6</v>
+      </c>
+      <c r="F21" s="27">
+        <v>7.9</v>
+      </c>
+      <c r="G21" s="27">
+        <v>6.4</v>
+      </c>
+      <c r="H21" s="27">
+        <v>6.6</v>
+      </c>
+      <c r="I21" s="27">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J21" s="27">
+        <v>9.5</v>
+      </c>
+      <c r="K21" s="27">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="L21" s="27">
+        <v>7.3</v>
+      </c>
+      <c r="M21" s="27">
+        <v>5.6</v>
+      </c>
+      <c r="N21" s="22">
+        <v>5.9</v>
+      </c>
+      <c r="O21" s="22">
+        <v>4.2</v>
+      </c>
+      <c r="P21" s="22">
+        <v>6.1</v>
+      </c>
+      <c r="Q21" s="22">
+        <v>4.2</v>
+      </c>
+      <c r="R21" s="22">
+        <v>6.6</v>
+      </c>
+      <c r="S21" s="22">
+        <v>4</v>
+      </c>
+      <c r="T21" s="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="27">
+        <v>3.4</v>
+      </c>
+      <c r="E22" s="27">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F22" s="27">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G22" s="27">
+        <v>2</v>
+      </c>
+      <c r="H22" s="27">
+        <v>2.8</v>
+      </c>
+      <c r="I22" s="27">
+        <v>2.4</v>
+      </c>
+      <c r="J22" s="27">
+        <v>2.9</v>
+      </c>
+      <c r="K22" s="27">
+        <v>3.3</v>
+      </c>
+      <c r="L22" s="27">
+        <v>1.5</v>
+      </c>
+      <c r="M22" s="27">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N22" s="22">
+        <v>1.6</v>
+      </c>
+      <c r="O22" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="P22" s="22">
+        <v>0.9</v>
+      </c>
+      <c r="Q22" s="22">
+        <v>1.6</v>
+      </c>
+      <c r="R22" s="22">
+        <v>1.7</v>
+      </c>
+      <c r="S22" s="22">
+        <v>1</v>
+      </c>
+      <c r="T22" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" s="30" customFormat="1">
+      <c r="A23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="25">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E23" s="25">
+        <v>4</v>
+      </c>
+      <c r="F23" s="25">
+        <v>7.5</v>
+      </c>
+      <c r="G23" s="25">
+        <v>7.8</v>
+      </c>
+      <c r="H23" s="25">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I23" s="25">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="J23" s="25">
+        <v>12.4</v>
+      </c>
+      <c r="K23" s="25">
+        <v>6.1</v>
+      </c>
+      <c r="L23" s="25">
+        <v>8.4</v>
+      </c>
+      <c r="M23" s="25">
+        <v>4.3</v>
+      </c>
+      <c r="N23" s="21">
+        <v>3.1</v>
+      </c>
+      <c r="O23" s="21">
+        <v>3.8</v>
+      </c>
+      <c r="P23" s="21">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="21">
+        <v>2.6</v>
+      </c>
+      <c r="R23" s="21">
+        <v>3.3</v>
+      </c>
+      <c r="S23" s="21">
+        <v>2.6</v>
+      </c>
+      <c r="T23" s="21">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="27">
+        <v>7.2</v>
+      </c>
+      <c r="E24" s="27">
+        <v>6.2</v>
+      </c>
+      <c r="F24" s="27">
+        <v>14</v>
+      </c>
+      <c r="G24" s="27">
+        <v>13</v>
+      </c>
+      <c r="H24" s="27">
+        <v>6.8</v>
+      </c>
+      <c r="I24" s="27">
+        <v>5.9</v>
+      </c>
+      <c r="J24" s="27">
+        <v>17.3</v>
+      </c>
+      <c r="K24" s="27">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="L24" s="27">
+        <v>14.3</v>
+      </c>
+      <c r="M24" s="27">
+        <v>7.8</v>
+      </c>
+      <c r="N24" s="22">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O24" s="22">
+        <v>6.1</v>
+      </c>
+      <c r="P24" s="22">
+        <v>6</v>
+      </c>
+      <c r="Q24" s="22">
+        <v>3.7</v>
+      </c>
+      <c r="R24" s="22">
+        <v>5.8</v>
+      </c>
+      <c r="S24" s="22">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="T24" s="22">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="27">
+        <v>2.7</v>
+      </c>
+      <c r="E25" s="27">
+        <v>1.8</v>
+      </c>
+      <c r="F25" s="27">
+        <v>0.9</v>
+      </c>
+      <c r="G25" s="27">
+        <v>2.6</v>
+      </c>
+      <c r="H25" s="27">
+        <v>3.4</v>
+      </c>
+      <c r="I25" s="27">
+        <v>4.2</v>
+      </c>
+      <c r="J25" s="27">
+        <v>7.5</v>
+      </c>
+      <c r="K25" s="27">
+        <v>2.5</v>
+      </c>
+      <c r="L25" s="27">
+        <v>2.4</v>
+      </c>
+      <c r="M25" s="27">
+        <v>0.8</v>
+      </c>
+      <c r="N25" s="22">
+        <v>3.9</v>
+      </c>
+      <c r="O25" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="P25" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q25" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="R25" s="22">
+        <v>0.7</v>
+      </c>
+      <c r="S25" s="22">
+        <v>0.7</v>
+      </c>
+      <c r="T25" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" s="30" customFormat="1">
+      <c r="A26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="25">
+        <v>15.8</v>
+      </c>
+      <c r="E26" s="25">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="F26" s="25">
+        <v>17.8</v>
+      </c>
+      <c r="G26" s="25">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="H26" s="25">
+        <v>17.2</v>
+      </c>
+      <c r="I26" s="25">
+        <v>20.5</v>
+      </c>
+      <c r="J26" s="25">
+        <v>14.2</v>
+      </c>
+      <c r="K26" s="25">
+        <v>14.4</v>
+      </c>
+      <c r="L26" s="25">
+        <v>13.8</v>
+      </c>
+      <c r="M26" s="25">
+        <v>16.7</v>
+      </c>
+      <c r="N26" s="21">
+        <v>15.2</v>
+      </c>
+      <c r="O26" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="P26" s="21">
+        <v>11.6</v>
+      </c>
+      <c r="Q26" s="21">
+        <v>13.1</v>
+      </c>
+      <c r="R26" s="21">
+        <v>15.2</v>
+      </c>
+      <c r="S26" s="21">
+        <v>10.6</v>
+      </c>
+      <c r="T26" s="21">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="27">
+        <v>25</v>
+      </c>
+      <c r="E27" s="27">
+        <v>28.6</v>
+      </c>
+      <c r="F27" s="27">
+        <v>28.8</v>
+      </c>
+      <c r="G27" s="27">
+        <v>32.6</v>
+      </c>
+      <c r="H27" s="27">
+        <v>27.3</v>
+      </c>
+      <c r="I27" s="27">
+        <v>31.3</v>
+      </c>
+      <c r="J27" s="27">
+        <v>22.8</v>
+      </c>
+      <c r="K27" s="27">
+        <v>24.5</v>
+      </c>
+      <c r="L27" s="27">
+        <v>21.5</v>
+      </c>
+      <c r="M27" s="27">
+        <v>27.9</v>
+      </c>
+      <c r="N27" s="22">
+        <v>25.1</v>
+      </c>
+      <c r="O27" s="22">
+        <v>24</v>
+      </c>
+      <c r="P27" s="22">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="Q27" s="22">
+        <v>20.6</v>
+      </c>
+      <c r="R27" s="22">
+        <v>24</v>
+      </c>
+      <c r="S27" s="22">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="T27" s="22">
+        <v>20.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="27">
+        <v>6.9</v>
+      </c>
+      <c r="E28" s="27">
+        <v>7.6</v>
+      </c>
+      <c r="F28" s="27">
+        <v>7.1</v>
+      </c>
+      <c r="G28" s="27">
+        <v>8</v>
+      </c>
+      <c r="H28" s="27">
+        <v>7.4</v>
+      </c>
+      <c r="I28" s="27">
+        <v>10</v>
+      </c>
+      <c r="J28" s="27">
+        <v>5.8</v>
+      </c>
+      <c r="K28" s="27">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L28" s="27">
+        <v>6.3</v>
+      </c>
+      <c r="M28" s="27">
+        <v>5.9</v>
+      </c>
+      <c r="N28" s="22">
+        <v>5.6</v>
+      </c>
+      <c r="O28" s="22">
+        <v>3.8</v>
+      </c>
+      <c r="P28" s="22">
+        <v>3.7</v>
+      </c>
+      <c r="Q28" s="22">
+        <v>5.9</v>
+      </c>
+      <c r="R28" s="22">
+        <v>6.6</v>
+      </c>
+      <c r="S28" s="22">
+        <v>2.6</v>
+      </c>
+      <c r="T28" s="22">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" s="30" customFormat="1">
+      <c r="A29" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="25">
+        <v>10.3</v>
+      </c>
+      <c r="E29" s="25">
+        <v>5.3</v>
+      </c>
+      <c r="F29" s="25">
+        <v>5.7</v>
+      </c>
+      <c r="G29" s="25">
+        <v>8.6</v>
+      </c>
+      <c r="H29" s="25">
+        <v>6.5</v>
+      </c>
+      <c r="I29" s="25">
+        <v>4.2</v>
+      </c>
+      <c r="J29" s="25">
+        <v>3.8</v>
+      </c>
+      <c r="K29" s="25">
+        <v>3.2</v>
+      </c>
+      <c r="L29" s="25">
+        <v>2.5</v>
+      </c>
+      <c r="M29" s="25">
+        <v>2.8</v>
+      </c>
+      <c r="N29" s="21">
+        <v>2.4</v>
+      </c>
+      <c r="O29" s="21">
+        <v>1.8</v>
+      </c>
+      <c r="P29" s="21">
+        <v>2.6</v>
+      </c>
+      <c r="Q29" s="21">
+        <v>1</v>
+      </c>
+      <c r="R29" s="21">
+        <v>2.4</v>
+      </c>
+      <c r="S29" s="21">
+        <v>2</v>
+      </c>
+      <c r="T29" s="21">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="27">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="E30" s="27">
+        <v>9.6</v>
+      </c>
+      <c r="F30" s="27">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G30" s="27">
+        <v>14.9</v>
+      </c>
+      <c r="H30" s="27">
+        <v>11.4</v>
+      </c>
+      <c r="I30" s="27">
+        <v>6.3</v>
+      </c>
+      <c r="J30" s="27">
+        <v>6.4</v>
+      </c>
+      <c r="K30" s="27">
+        <v>5.3</v>
+      </c>
+      <c r="L30" s="27">
+        <v>3.8</v>
+      </c>
+      <c r="M30" s="27">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="N30" s="22">
+        <v>3.7</v>
+      </c>
+      <c r="O30" s="22">
+        <v>3.2</v>
+      </c>
+      <c r="P30" s="22">
+        <v>4.7</v>
+      </c>
+      <c r="Q30" s="22">
+        <v>1.2</v>
+      </c>
+      <c r="R30" s="22">
+        <v>3.5</v>
+      </c>
+      <c r="S30" s="22">
+        <v>3.3</v>
+      </c>
+      <c r="T30" s="22">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="27">
+        <v>4.3</v>
+      </c>
+      <c r="E31" s="27">
+        <v>1.6</v>
+      </c>
+      <c r="F31" s="27">
+        <v>3.6</v>
+      </c>
+      <c r="G31" s="27">
+        <v>3.1</v>
+      </c>
+      <c r="H31" s="27">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I31" s="27">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J31" s="27">
+        <v>1.4</v>
+      </c>
+      <c r="K31" s="27">
+        <v>1.4</v>
+      </c>
+      <c r="L31" s="27">
+        <v>1.4</v>
+      </c>
+      <c r="M31" s="27">
+        <v>1</v>
+      </c>
+      <c r="N31" s="22">
+        <v>1.3</v>
+      </c>
+      <c r="O31" s="22">
+        <v>0.6</v>
+      </c>
+      <c r="P31" s="22">
+        <v>0.7</v>
+      </c>
+      <c r="Q31" s="22">
+        <v>0.9</v>
+      </c>
+      <c r="R31" s="22">
+        <v>1.4</v>
+      </c>
+      <c r="S31" s="22">
+        <v>1</v>
+      </c>
+      <c r="T31" s="22">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" s="30" customFormat="1">
+      <c r="A32" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="25">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E32" s="25">
+        <v>3.9</v>
+      </c>
+      <c r="F32" s="25">
+        <v>4.3</v>
+      </c>
+      <c r="G32" s="25">
+        <v>1.6</v>
+      </c>
+      <c r="H32" s="25">
+        <v>1.6</v>
+      </c>
+      <c r="I32" s="25">
+        <v>2.7</v>
+      </c>
+      <c r="J32" s="25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K32" s="25">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L32" s="25">
+        <v>1.8</v>
+      </c>
+      <c r="M32" s="25">
+        <v>2.5</v>
+      </c>
+      <c r="N32" s="21">
+        <v>2.5</v>
+      </c>
+      <c r="O32" s="21">
+        <v>1.7</v>
+      </c>
+      <c r="P32" s="21">
+        <v>2.9</v>
+      </c>
+      <c r="Q32" s="21">
+        <v>1.3</v>
+      </c>
+      <c r="R32" s="21">
+        <v>0.6</v>
+      </c>
+      <c r="S32" s="21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T32" s="21">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="A33" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="27">
+        <v>2.4</v>
+      </c>
+      <c r="E33" s="27">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F33" s="27">
+        <v>7.2</v>
+      </c>
+      <c r="G33" s="27">
+        <v>2.4</v>
+      </c>
+      <c r="H33" s="27">
+        <v>2.4</v>
+      </c>
+      <c r="I33" s="27">
+        <v>4.8</v>
+      </c>
+      <c r="J33" s="27">
+        <v>0.8</v>
+      </c>
+      <c r="K33" s="27">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L33" s="27">
+        <v>3</v>
+      </c>
+      <c r="M33" s="27">
+        <v>5.2</v>
+      </c>
+      <c r="N33" s="22">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="O33" s="22">
+        <v>2.8</v>
+      </c>
+      <c r="P33" s="22">
+        <v>6.1</v>
+      </c>
+      <c r="Q33" s="22">
+        <v>1.3</v>
+      </c>
+      <c r="R33" s="22">
+        <v>1.3</v>
+      </c>
+      <c r="S33" s="22">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T33" s="22">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="15.75" thickBot="1">
+      <c r="A34" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E34" s="17">
+        <v>3</v>
+      </c>
+      <c r="F34" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="G34" s="17">
+        <v>0.7</v>
+      </c>
+      <c r="H34" s="17">
+        <v>0.8</v>
+      </c>
+      <c r="I34" s="17">
+        <v>0.7</v>
+      </c>
+      <c r="J34" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="K34" s="17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L34" s="17">
+        <v>0.7</v>
+      </c>
+      <c r="M34" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="N34" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="O34" s="20">
+        <v>0.7</v>
+      </c>
+      <c r="P34" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q34" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="R34" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="S34" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="T34" s="20">
+        <v>1.7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>